<commit_message>
Assigned ADC inputs and I2C expansion bus.
</commit_message>
<xml_diff>
--- a/PinAssignment.xlsx
+++ b/PinAssignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\CordicVCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D76F24-0FD0-4876-93F2-FFE41D2E50AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124DE233-626C-4A7C-A23E-29DA41124C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21555" yWindow="7860" windowWidth="21600" windowHeight="28035" activeTab="1" xr2:uid="{DAF99840-0FB4-4B5C-8F3C-2FDCEC42588D}"/>
+    <workbookView xWindow="21465" yWindow="6210" windowWidth="21600" windowHeight="28035" activeTab="1" xr2:uid="{DAF99840-0FB4-4B5C-8F3C-2FDCEC42588D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
   <si>
     <t>PA4</t>
   </si>
@@ -614,6 +614,42 @@
   </si>
   <si>
     <t>RESET</t>
+  </si>
+  <si>
+    <t>ADC12</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>CV1A</t>
+  </si>
+  <si>
+    <t>CV1B</t>
+  </si>
+  <si>
+    <t>CV2A</t>
+  </si>
+  <si>
+    <t>CV2B</t>
+  </si>
+  <si>
+    <t>CV3A</t>
+  </si>
+  <si>
+    <t>CV3B</t>
+  </si>
+  <si>
+    <t>CV4A</t>
+  </si>
+  <si>
+    <t>CV4B</t>
+  </si>
+  <si>
+    <t>I2C</t>
   </si>
 </sst>
 </file>
@@ -642,7 +678,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,6 +733,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -719,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -760,6 +808,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1735,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0CFA78-0A62-4007-8D89-5CCC3EA1AC17}">
-  <dimension ref="B3:P51"/>
+  <dimension ref="B3:S58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,9 +2022,8 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="str">
-        <f t="shared" ref="B11:B14" si="0">L11</f>
-        <v>ADC12_IN1</v>
+      <c r="B11" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="C11" s="10">
         <v>8</v>
@@ -2010,9 +2063,8 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>ADC12_IN2</v>
+      <c r="B12" s="18" t="s">
+        <v>198</v>
       </c>
       <c r="C12" s="10">
         <v>9</v>
@@ -2049,9 +2101,8 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>ADC1_IN3</v>
+      <c r="B13" s="18" t="s">
+        <v>199</v>
       </c>
       <c r="C13" s="10">
         <v>10</v>
@@ -2091,9 +2142,8 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="str">
-        <f>L14</f>
-        <v>ADC1_IN4</v>
+      <c r="B14" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="C14" s="10">
         <v>11</v>
@@ -2130,10 +2180,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="str">
-        <f>L15</f>
-        <v>ADC2_IN17</v>
-      </c>
+      <c r="B15" s="12"/>
       <c r="C15" s="10">
         <v>12</v>
       </c>
@@ -2204,9 +2251,8 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="str">
-        <f>L17</f>
-        <v>ADC2_IN3</v>
+      <c r="B17" s="18" t="s">
+        <v>200</v>
       </c>
       <c r="C17" s="11">
         <v>14</v>
@@ -2275,9 +2321,8 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="str">
-        <f>L19</f>
-        <v>ADC1_IN15</v>
+      <c r="B19" s="18" t="s">
+        <v>203</v>
       </c>
       <c r="C19" s="11">
         <v>16</v>
@@ -2349,10 +2394,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="str">
-        <f t="shared" ref="B21:B28" si="1">L21</f>
-        <v>ADC2_IN12</v>
-      </c>
+      <c r="B21" s="12"/>
       <c r="C21" s="11">
         <v>18</v>
       </c>
@@ -2468,10 +2510,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>OPAMP3_VINM</v>
-      </c>
+      <c r="B25" s="12"/>
       <c r="C25" s="11">
         <v>22</v>
       </c>
@@ -2552,9 +2591,8 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>ADC12_IN14</v>
+      <c r="B28" s="18" t="s">
+        <v>202</v>
       </c>
       <c r="C28" s="10">
         <v>25</v>
@@ -2640,10 +2678,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="str">
-        <f t="shared" ref="B31:B34" si="2">L31</f>
-        <v>ADC1_IN5</v>
-      </c>
+      <c r="B31" s="12"/>
       <c r="C31" s="10">
         <v>28</v>
       </c>
@@ -2673,9 +2708,8 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>ADC2_IN15</v>
+      <c r="B32" s="18" t="s">
+        <v>204</v>
       </c>
       <c r="C32" s="10">
         <v>29</v>
@@ -2703,7 +2737,9 @@
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
+      <c r="B33" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="C33" s="10">
         <v>30</v>
       </c>
@@ -2730,7 +2766,9 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="C34" s="10">
         <v>31</v>
       </c>
@@ -3156,7 +3194,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>158</v>
       </c>
@@ -3185,7 +3223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B50" s="16"/>
       <c r="C50" s="11">
         <v>47</v>
@@ -3212,7 +3250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B51" s="16"/>
       <c r="C51" s="11">
         <v>48</v>
@@ -3237,6 +3275,66 @@
       </c>
       <c r="L51" s="9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
+        <v>194</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L57" t="s">
+        <v>195</v>
+      </c>
+      <c r="M57">
+        <v>3</v>
+      </c>
+      <c r="N57">
+        <v>4</v>
+      </c>
+      <c r="O57">
+        <v>5</v>
+      </c>
+      <c r="P57">
+        <v>11</v>
+      </c>
+      <c r="Q57">
+        <v>12</v>
+      </c>
+      <c r="R57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
+        <v>196</v>
+      </c>
+      <c r="M58">
+        <v>3</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+      <c r="O58">
+        <v>12</v>
+      </c>
+      <c r="P58">
+        <v>13</v>
+      </c>
+      <c r="Q58">
+        <v>14</v>
+      </c>
+      <c r="R58">
+        <v>15</v>
+      </c>
+      <c r="S58">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV inputs, including spice checks.
</commit_message>
<xml_diff>
--- a/PinAssignment.xlsx
+++ b/PinAssignment.xlsx
@@ -8,14 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\CordicVCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9D3FBD-9AF0-4031-9FAB-C76FBAC16997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1CB233-5446-497E-8EDF-5583CD513B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21465" yWindow="6210" windowWidth="21600" windowHeight="28035" activeTab="1" xr2:uid="{DAF99840-0FB4-4B5C-8F3C-2FDCEC42588D}"/>
+    <workbookView xWindow="17205" yWindow="15300" windowWidth="21600" windowHeight="28035" activeTab="2" xr2:uid="{DAF99840-0FB4-4B5C-8F3C-2FDCEC42588D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet3!$H$10:$H$11</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet3!$H$20</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">2.9</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="220">
   <si>
     <t>PA4</t>
   </si>
@@ -650,13 +680,59 @@
   </si>
   <si>
     <t>I2C</t>
+  </si>
+  <si>
+    <t>Rf</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>Rref</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>I(Rref)</t>
+  </si>
+  <si>
+    <t>Vmin</t>
+  </si>
+  <si>
+    <t>Vmax</t>
+  </si>
+  <si>
+    <t>I(Rgmin)</t>
+  </si>
+  <si>
+    <t>I(Rgmax)</t>
+  </si>
+  <si>
+    <t>I(Rfmin)</t>
+  </si>
+  <si>
+    <t>I(Rfmax)</t>
+  </si>
+  <si>
+    <t>V/OCT</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>0-5V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +752,34 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -764,10 +868,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -816,8 +921,22 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1791,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0CFA78-0A62-4007-8D89-5CCC3EA1AC17}">
   <dimension ref="B3:S58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,4 +3460,315 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B36A00-F8AB-4AD2-8006-DF1A653A4978}">
+  <dimension ref="C6:H20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="23">
+        <v>-3</v>
+      </c>
+      <c r="E7" s="24">
+        <f>D7</f>
+        <v>-3</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
+        <f>G7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="23">
+        <v>6</v>
+      </c>
+      <c r="E8" s="24">
+        <f>D8</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="23">
+        <v>5</v>
+      </c>
+      <c r="H8" s="24">
+        <f>G8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="22">
+        <v>102413.60973314675</v>
+      </c>
+      <c r="E9" s="22">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="22">
+        <v>100000</v>
+      </c>
+      <c r="H9" s="22">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="22">
+        <v>33000</v>
+      </c>
+      <c r="E10" s="25">
+        <f>D10</f>
+        <v>33000</v>
+      </c>
+      <c r="G10" s="22">
+        <v>57999.95336225965</v>
+      </c>
+      <c r="H10" s="22">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="22">
+        <v>170689.46344817404</v>
+      </c>
+      <c r="E11" s="22">
+        <v>169000</v>
+      </c>
+      <c r="G11" s="22">
+        <v>199999.68545147291</v>
+      </c>
+      <c r="H11" s="22">
+        <v>199999.68545147291</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="21">
+        <v>-10</v>
+      </c>
+      <c r="E12" s="21">
+        <v>-10</v>
+      </c>
+      <c r="G12" s="21">
+        <v>-10</v>
+      </c>
+      <c r="H12" s="21">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="20">
+        <f>D7/D9</f>
+        <v>-2.9292981741556885E-5</v>
+      </c>
+      <c r="E13" s="20">
+        <f>E7/E9</f>
+        <v>-3.0000000000000001E-5</v>
+      </c>
+      <c r="G13" s="20">
+        <f>G7/G9</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <f>H7/H9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="20">
+        <f>D8/D9</f>
+        <v>5.8585963483113769E-5</v>
+      </c>
+      <c r="E14" s="20">
+        <f>E8/E9</f>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="G14" s="20">
+        <f>G8/G9</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="H14" s="20">
+        <f>H8/H9</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="20">
+        <f>D12/D11</f>
+        <v>-5.85859243914975E-5</v>
+      </c>
+      <c r="E15" s="20">
+        <f>E12/E11</f>
+        <v>-5.9171597633136094E-5</v>
+      </c>
+      <c r="G15" s="20">
+        <f>G12/G11</f>
+        <v>-5.0000078637255449E-5</v>
+      </c>
+      <c r="H15" s="20">
+        <f>H12/H11</f>
+        <v>-5.0000078637255449E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" s="20">
+        <f>-(D13+D15)</f>
+        <v>8.7878906133054388E-5</v>
+      </c>
+      <c r="E16" s="20">
+        <f>-(E13+E15)</f>
+        <v>8.9171597633136098E-5</v>
+      </c>
+      <c r="G16" s="20">
+        <f>-(G13+G15)</f>
+        <v>5.0000078637255449E-5</v>
+      </c>
+      <c r="H16" s="20">
+        <f>-(H13+H15)</f>
+        <v>5.0000078637255449E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="20">
+        <f>-(D14+D15)</f>
+        <v>-3.9091616269438904E-11</v>
+      </c>
+      <c r="E17" s="20">
+        <f>-(E14+E15)</f>
+        <v>-8.2840236686390742E-7</v>
+      </c>
+      <c r="G17" s="20">
+        <f>-(G14+G15)</f>
+        <v>7.8637255446201409E-11</v>
+      </c>
+      <c r="H17" s="20">
+        <f>-(H14+H15)</f>
+        <v>7.8637255446201409E-11</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="21">
+        <f>D16*D10</f>
+        <v>2.9000039023907949</v>
+      </c>
+      <c r="E18" s="21">
+        <f>E16*E10</f>
+        <v>2.9426627218934911</v>
+      </c>
+      <c r="G18" s="21">
+        <f>G16*G10</f>
+        <v>2.9000022290701311</v>
+      </c>
+      <c r="H18" s="21">
+        <f>H16*H10</f>
+        <v>2.8000044036863052</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="21">
+        <f>D17*D10</f>
+        <v>-1.2900233368914838E-6</v>
+      </c>
+      <c r="E19" s="21">
+        <f>E17*E10</f>
+        <v>-2.7337278106508944E-2</v>
+      </c>
+      <c r="G19" s="21">
+        <f>G17*G10</f>
+        <v>4.5609571484157805E-6</v>
+      </c>
+      <c r="H19" s="21">
+        <f>H17*H10</f>
+        <v>4.4036863049872789E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="20">
+        <f>(D18-2.9)^2+D19^2</f>
+        <v>1.689281412625095E-11</v>
+      </c>
+      <c r="E20" s="20">
+        <f>(E18-2.9)^2+E19^2</f>
+        <v>2.5674346136339852E-3</v>
+      </c>
+      <c r="G20" s="20">
+        <f>(G18-2.9)^2+G19^2</f>
+        <v>2.5771083759240544E-11</v>
+      </c>
+      <c r="H20" s="20">
+        <f>(H18-2.9)^2+H19^2</f>
+        <v>9.9991193015238466E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>